<commit_message>
Trying dask for parallelization
</commit_message>
<xml_diff>
--- a/data_and_models/Model, parameters and uncertainty.xlsx
+++ b/data_and_models/Model, parameters and uncertainty.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andrea\OneDrive - University College London\S4CE\LCA\GSA\Geothermal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andrea\OneDrive - University College London\S4CE\GSA\Geothermal\data_and_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19430" windowHeight="10430" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Simplified models" sheetId="8" r:id="rId1"/>
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="0" shapeId="0">
+    <comment ref="G6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0" shapeId="0">
+    <comment ref="H19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -422,7 +422,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="247">
   <si>
     <t>Remarks</t>
   </si>
@@ -1157,6 +1157,30 @@
   <si>
     <t>Lognormal distribution. Scipy: Shape = 0.98; scale=0.077.</t>
   </si>
+  <si>
+    <t>0-260</t>
+  </si>
+  <si>
+    <t>0=1583</t>
+  </si>
+  <si>
+    <t>From Geothermal power database</t>
+  </si>
+  <si>
+    <t>0-</t>
+  </si>
+  <si>
+    <t>Triangular distribution, by plants name. Scipy: Shape~1.15; scale~38.80; loc=0</t>
+  </si>
+  <si>
+    <t>Triangular distribution, by fields name.Scipy: Shape~1.48; scale~65.32; loc=0</t>
+  </si>
+  <si>
+    <t>Triangular distribution, by plants name. Scipy: Shape~1.17; scale~10.01; loc=0</t>
+  </si>
+  <si>
+    <t>Triangular distribution, by fields name.Scipy: Shape~1.17; scale~12.11; loc=0</t>
+  </si>
 </sst>
 </file>
 
@@ -1293,7 +1317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1367,13 +1391,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1569,6 +1602,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1592,6 +1631,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1735,8 +1777,8 @@
       <xdr:rowOff>44903</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="16314965" cy="666751"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -5036,7 +5078,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -38484,12 +38526,12 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="255.5703125" style="40" customWidth="1"/>
+    <col min="1" max="1" width="255.54296875" style="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="70"/>
     </row>
   </sheetData>
@@ -38508,72 +38550,72 @@
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="255.5703125" style="40" customWidth="1"/>
-    <col min="2" max="2" width="255.28515625" style="40" customWidth="1"/>
+    <col min="1" max="1" width="255.54296875" style="40" customWidth="1"/>
+    <col min="2" max="2" width="255.26953125" style="40" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
-    <col min="9" max="9" width="37.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1796875" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" customWidth="1"/>
+    <col min="8" max="8" width="18.1796875" customWidth="1"/>
+    <col min="9" max="9" width="37.453125" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.54296875" customWidth="1"/>
+    <col min="13" max="13" width="14.54296875" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="12:16" x14ac:dyDescent="0.35">
       <c r="N1" s="37"/>
     </row>
-    <row r="2" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M2" s="37"/>
       <c r="O2" s="37"/>
       <c r="P2" s="38"/>
     </row>
-    <row r="3" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="12:16" x14ac:dyDescent="0.35">
       <c r="N3" s="39"/>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="12:16" x14ac:dyDescent="0.35">
       <c r="N4" s="39"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="12:16" x14ac:dyDescent="0.35">
       <c r="N5" s="39"/>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="12:16" x14ac:dyDescent="0.35">
       <c r="N6" s="39"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="12:16" x14ac:dyDescent="0.35">
       <c r="N7" s="39"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="12:16" x14ac:dyDescent="0.35">
       <c r="N8" s="39"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="12:16" x14ac:dyDescent="0.35">
       <c r="N9" s="39"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="12:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="12:16" x14ac:dyDescent="0.35">
       <c r="N10" s="39"/>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="12:16" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="12:16" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L11" s="6"/>
     </row>
-    <row r="21" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="3:17" s="40" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" ht="35.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" ht="13.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="3:17" s="40" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35"/>
@@ -38590,7 +38632,7 @@
       <c r="P35"/>
       <c r="Q35"/>
     </row>
-    <row r="36" spans="3:17" s="40" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:17" s="40" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
@@ -38607,7 +38649,7 @@
       <c r="P36"/>
       <c r="Q36"/>
     </row>
-    <row r="37" spans="3:17" s="40" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:17" s="40" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
@@ -38624,7 +38666,7 @@
       <c r="P37"/>
       <c r="Q37"/>
     </row>
-    <row r="38" spans="3:17" s="40" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:17" s="40" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
@@ -38641,7 +38683,7 @@
       <c r="P38"/>
       <c r="Q38"/>
     </row>
-    <row r="39" spans="3:17" s="40" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:17" s="40" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C39"/>
       <c r="D39"/>
       <c r="E39"/>
@@ -38658,7 +38700,7 @@
       <c r="P39"/>
       <c r="Q39"/>
     </row>
-    <row r="40" spans="3:17" s="40" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:17" s="40" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C40"/>
       <c r="D40"/>
       <c r="E40"/>
@@ -38675,7 +38717,7 @@
       <c r="P40"/>
       <c r="Q40"/>
     </row>
-    <row r="41" spans="3:17" s="40" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:17" s="40" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C41"/>
       <c r="D41"/>
       <c r="E41"/>
@@ -38692,7 +38734,7 @@
       <c r="P41"/>
       <c r="Q41"/>
     </row>
-    <row r="42" spans="3:17" s="40" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:17" s="40" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C42"/>
       <c r="D42"/>
       <c r="E42"/>
@@ -38709,7 +38751,7 @@
       <c r="P42"/>
       <c r="Q42"/>
     </row>
-    <row r="43" spans="3:17" s="40" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:17" s="40" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C43"/>
       <c r="D43"/>
       <c r="E43"/>
@@ -38726,7 +38768,7 @@
       <c r="P43"/>
       <c r="Q43"/>
     </row>
-    <row r="44" spans="3:17" s="40" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:17" s="40" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C44"/>
       <c r="D44"/>
       <c r="E44"/>
@@ -38743,7 +38785,7 @@
       <c r="P44"/>
       <c r="Q44"/>
     </row>
-    <row r="45" spans="3:17" s="40" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:17" s="40" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C45"/>
       <c r="D45"/>
       <c r="E45"/>
@@ -38760,7 +38802,7 @@
       <c r="P45"/>
       <c r="Q45"/>
     </row>
-    <row r="46" spans="3:17" s="40" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:17" s="40" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C46"/>
       <c r="D46"/>
       <c r="E46"/>
@@ -38777,7 +38819,7 @@
       <c r="P46"/>
       <c r="Q46"/>
     </row>
-    <row r="85" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="17:17" x14ac:dyDescent="0.35">
       <c r="Q85" s="5"/>
     </row>
   </sheetData>
@@ -38796,22 +38838,22 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.7109375" customWidth="1"/>
+    <col min="1" max="1" width="44.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -38824,27 +38866,27 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" customWidth="1"/>
     <col min="2" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="63.28515625" customWidth="1"/>
-    <col min="6" max="6" width="58.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="56.42578125" customWidth="1"/>
-    <col min="9" max="9" width="70.140625" customWidth="1"/>
-    <col min="10" max="10" width="48.5703125" customWidth="1"/>
-    <col min="13" max="13" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" customWidth="1"/>
+    <col min="5" max="5" width="63.26953125" customWidth="1"/>
+    <col min="6" max="6" width="58.26953125" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
+    <col min="8" max="8" width="56.453125" customWidth="1"/>
+    <col min="9" max="9" width="70.1796875" customWidth="1"/>
+    <col min="10" max="10" width="48.54296875" customWidth="1"/>
+    <col min="13" max="13" width="36.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="37" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="37" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="73" t="s">
         <v>155</v>
       </c>
@@ -38865,7 +38907,7 @@
       <c r="H1" s="72"/>
       <c r="I1" s="72"/>
     </row>
-    <row r="2" spans="1:15" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="73"/>
       <c r="B2" s="73"/>
       <c r="C2" s="73"/>
@@ -38897,14 +38939,14 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="76" t="s">
         <v>167</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -38929,266 +38971,248 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="71"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="F4" s="75" t="s">
+        <v>241</v>
+      </c>
+      <c r="G4" s="85" t="s">
+        <v>242</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>245</v>
+      </c>
+      <c r="I4" s="75" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="71"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="E5" s="49" t="s">
+        <v>244</v>
+      </c>
+      <c r="F5" s="75"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="49" t="s">
+        <v>246</v>
+      </c>
+      <c r="I5" s="75"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E6" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F6" t="s">
         <v>103</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H6" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I6" t="s">
         <v>91</v>
       </c>
-      <c r="M4" s="33" t="s">
+      <c r="M6" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="N4">
-        <f>N$2/$M4</f>
+      <c r="N6">
+        <f>N$2/$M6</f>
         <v>5</v>
       </c>
-      <c r="O4">
-        <f>O$2/$M4</f>
+      <c r="O6">
+        <f>O$2/$M6</f>
         <v>32.5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>81</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>169</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="49" t="s">
+      <c r="E7" s="49" t="s">
         <v>226</v>
       </c>
-      <c r="F5" s="69" t="s">
+      <c r="F7" s="69" t="s">
         <v>232</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H7" s="49" t="s">
         <v>226</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I7" t="s">
         <v>88</v>
       </c>
-      <c r="M5" s="23">
+      <c r="M7" s="23">
         <v>16</v>
       </c>
-      <c r="N5">
-        <f>N$2/$M5</f>
+      <c r="N7">
+        <f>N$2/$M7</f>
         <v>1.25</v>
       </c>
-      <c r="O5">
-        <f>O$2/$M5</f>
+      <c r="O7">
+        <f>O$2/$M7</f>
         <v>8.125</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>86</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>170</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E8" s="49" t="s">
         <v>187</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F8" t="s">
         <v>83</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H8" s="49" t="s">
         <v>187</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>97</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>171</v>
       </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="3" t="s">
+      <c r="D9" s="47"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="H7" s="49" t="s">
+      <c r="H9" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="10" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>62</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>182</v>
       </c>
-      <c r="D8" s="62" t="s">
+      <c r="D10" s="62" t="s">
         <v>217</v>
       </c>
-      <c r="E8" s="64" t="s">
+      <c r="E10" s="64" t="s">
         <v>222</v>
       </c>
-      <c r="F8" s="63" t="s">
+      <c r="F10" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="G8" s="65" t="s">
+      <c r="G10" s="65" t="s">
         <v>217</v>
       </c>
-      <c r="H8" s="66" t="s">
+      <c r="H10" s="66" t="s">
         <v>221</v>
       </c>
-      <c r="I8" s="67" t="s">
+      <c r="I10" s="67" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>72</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>172</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="E9" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" t="s">
-        <v>234</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="H9" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="I9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>173</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" t="s">
-        <v>114</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="I10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B11" t="s">
-        <v>188</v>
-      </c>
-      <c r="C11" t="s">
-        <v>174</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>189</v>
       </c>
       <c r="E11" s="49" t="s">
         <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>114</v>
+        <v>234</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="H11" s="49" t="s">
         <v>90</v>
       </c>
       <c r="I11" t="s">
-        <v>119</v>
+        <v>198</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E12" s="49" t="s">
         <v>90</v>
@@ -39196,314 +39220,377 @@
       <c r="F12" t="s">
         <v>114</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>116</v>
+      <c r="G12" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="H12" s="49" t="s">
         <v>90</v>
       </c>
       <c r="I12" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="C13" t="s">
-        <v>175</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>112</v>
+        <v>174</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>189</v>
       </c>
       <c r="E13" s="49" t="s">
         <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>120</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="H13" s="49" t="s">
         <v>90</v>
       </c>
       <c r="I13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H15" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="I15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>176</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E16" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F16" t="s">
         <v>121</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="H16" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I16" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="17" spans="1:10" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>193</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>177</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="E15" s="49" t="s">
+      <c r="E17" s="49" t="s">
         <v>238</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F17" t="s">
         <v>118</v>
       </c>
-      <c r="G15" s="36"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="36"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="56"/>
-      <c r="H16" s="49"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="56"/>
+      <c r="H18" s="49"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>106</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>178</v>
       </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="I17" t="s">
-        <v>109</v>
-      </c>
-      <c r="J17" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" t="s">
-        <v>107</v>
-      </c>
-      <c r="C18" t="s">
-        <v>216</v>
-      </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="I18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="B19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" t="s">
-        <v>184</v>
-      </c>
       <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
+      <c r="E19" s="52"/>
       <c r="F19" s="36"/>
       <c r="G19" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H19" s="23" t="s">
         <v>90</v>
       </c>
+      <c r="I19" t="s">
+        <v>109</v>
+      </c>
+      <c r="J19" t="s">
+        <v>180</v>
+      </c>
     </row>
-    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" t="s">
+        <v>216</v>
+      </c>
+      <c r="D20" s="36"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="I20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="39" t="s">
         <v>201</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="D21" s="58" t="s">
+      <c r="D23" s="58" t="s">
         <v>202</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="F21" s="49" t="s">
+      <c r="F23" s="49" t="s">
         <v>220</v>
       </c>
-      <c r="G21" s="61"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="F22" s="71" t="s">
+      <c r="F24" s="71" t="s">
         <v>212</v>
       </c>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
     </row>
-    <row r="23" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+    <row r="25" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="22" t="s">
         <v>204</v>
-      </c>
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" t="s">
-        <v>207</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F23" s="71"/>
-      <c r="G23" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="I23" s="74" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" t="s">
-        <v>208</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="F24" s="71"/>
-      <c r="G24" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="I24" s="74"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>206</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>218</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F25" s="71"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
+      <c r="G25" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I25" s="74" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D26" s="5"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>208</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F26" s="71"/>
+      <c r="G26" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="I26" s="74"/>
     </row>
-    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="C27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F27" s="71"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="F22:F25"/>
+  <mergeCells count="12">
+    <mergeCell ref="F24:F27"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="I4:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -39520,16 +39607,16 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="69.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.54296875" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" customWidth="1"/>
+    <col min="8" max="8" width="15.1796875" customWidth="1"/>
+    <col min="9" max="9" width="69.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="41" t="s">
         <v>156</v>
       </c>
@@ -39549,7 +39636,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>157</v>
       </c>
@@ -39569,7 +39656,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -39589,7 +39676,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>164</v>
       </c>
@@ -39609,7 +39696,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H6" s="22" t="s">
         <v>130</v>
       </c>
@@ -39617,7 +39704,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H7" s="22" t="s">
         <v>131</v>
       </c>
@@ -39625,7 +39712,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="37"/>
       <c r="B8" s="37"/>
       <c r="C8" s="45"/>
@@ -39637,7 +39724,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H9" s="22" t="s">
         <v>153</v>
       </c>
@@ -39645,7 +39732,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H10" s="22" t="s">
         <v>194</v>
       </c>
@@ -39653,7 +39740,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H11" t="s">
         <v>133</v>
       </c>
@@ -39661,7 +39748,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H12" t="s">
         <v>135</v>
       </c>
@@ -39669,7 +39756,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H13" s="22" t="s">
         <v>137</v>
       </c>
@@ -39677,7 +39764,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H14" s="22" t="s">
         <v>139</v>
       </c>
@@ -39685,7 +39772,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H15" s="42" t="s">
         <v>141</v>
       </c>
@@ -39693,7 +39780,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H16" s="59" t="s">
         <v>143</v>
       </c>
@@ -39701,7 +39788,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H17" s="43" t="s">
         <v>145</v>
       </c>
@@ -39709,7 +39796,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H18" s="42" t="s">
         <v>235</v>
       </c>
@@ -39717,7 +39804,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H19" s="42" t="s">
         <v>236</v>
       </c>
@@ -39725,7 +39812,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H20" t="s">
         <v>237</v>
       </c>
@@ -39748,56 +39835,56 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="9" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="8" max="9" width="15.54296875" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" customWidth="1"/>
+    <col min="15" max="15" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:15" s="6" customFormat="1" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80" t="s">
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80" t="s">
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="80"/>
+      <c r="N1" s="82"/>
       <c r="O1" s="20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75"/>
-      <c r="B2" s="75"/>
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
       <c r="C2" s="29" t="s">
         <v>29</v>
       </c>
@@ -39838,7 +39925,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -39846,7 +39933,7 @@
       <c r="L3" s="32"/>
       <c r="N3" s="32"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>4</v>
       </c>
@@ -39856,16 +39943,16 @@
       <c r="C4" s="7">
         <v>2</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="81" t="s">
+      <c r="F4" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="G4" s="79" t="s">
         <v>41</v>
       </c>
       <c r="H4" s="24" t="s">
@@ -39877,21 +39964,21 @@
       <c r="J4" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="81" t="s">
+      <c r="K4" s="83" t="s">
         <v>39</v>
       </c>
       <c r="L4" s="28">
         <v>14</v>
       </c>
-      <c r="M4" s="76" t="s">
+      <c r="M4" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="77"/>
+      <c r="N4" s="79"/>
       <c r="O4" s="1">
         <v>7.2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>3</v>
       </c>
@@ -39901,10 +39988,10 @@
       <c r="C5" s="7">
         <v>100</v>
       </c>
-      <c r="D5" s="82"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="77"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="79"/>
       <c r="H5" s="27" t="s">
         <v>44</v>
       </c>
@@ -39914,17 +40001,17 @@
       <c r="J5" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="K5" s="81"/>
+      <c r="K5" s="83"/>
       <c r="L5" s="28">
         <v>309</v>
       </c>
-      <c r="M5" s="76"/>
-      <c r="N5" s="77"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="79"/>
       <c r="O5" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>45</v>
       </c>
@@ -39934,10 +40021,10 @@
       <c r="C6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="77"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="79"/>
       <c r="H6" s="27" t="s">
         <v>46</v>
       </c>
@@ -39947,17 +40034,17 @@
       <c r="J6" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="81"/>
+      <c r="K6" s="83"/>
       <c r="L6" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="76"/>
-      <c r="N6" s="77"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="79"/>
       <c r="O6" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>6</v>
       </c>
@@ -39967,12 +40054,12 @@
       <c r="C7" s="7">
         <v>9.3000000000000007</v>
       </c>
-      <c r="D7" s="82"/>
+      <c r="D7" s="84"/>
       <c r="E7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="81"/>
-      <c r="G7" s="77"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="79"/>
       <c r="H7" s="18">
         <v>0.67</v>
       </c>
@@ -39988,15 +40075,15 @@
       <c r="L7" s="12">
         <v>0.5</v>
       </c>
-      <c r="M7" s="78" t="s">
+      <c r="M7" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="N7" s="79"/>
+      <c r="N7" s="81"/>
       <c r="O7" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>80</v>
       </c>
@@ -40014,7 +40101,7 @@
       <c r="N8" s="12"/>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>58</v>
       </c>
@@ -40061,7 +40148,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>11</v>
       </c>
@@ -40105,7 +40192,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
         <v>1</v>
       </c>
@@ -40141,7 +40228,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
         <v>2</v>
       </c>
@@ -40188,7 +40275,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>10</v>
       </c>
@@ -40233,7 +40320,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
         <v>81</v>
       </c>
@@ -40276,7 +40363,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
simplified models coefficients with thresholds
</commit_message>
<xml_diff>
--- a/data_and_models/Model, parameters and uncertainty.xlsx
+++ b/data_and_models/Model, parameters and uncertainty.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simplified models" sheetId="8" r:id="rId1"/>
@@ -6063,8 +6063,8 @@
       <xdr:rowOff>9712</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="545406" cy="183192"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -6189,7 +6189,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9">
@@ -6266,8 +6266,8 @@
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="14690538" cy="681084"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -9484,7 +9484,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -24681,8 +24681,8 @@
       <xdr:rowOff>142972</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1261307" cy="176972"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="40" name="TextBox 39">
@@ -24929,7 +24929,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="40" name="TextBox 39">
@@ -28437,9 +28437,9 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>169937</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="17882092" cy="479427"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="17882092" cy="502382"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="33" name="TextBox 32">
@@ -28453,8 +28453,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="215409" y="2017210"/>
-              <a:ext cx="17882092" cy="479427"/>
+              <a:off x="215409" y="2074937"/>
+              <a:ext cx="17882092" cy="502382"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -28659,7 +28659,7 @@
                                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
-                              <m:t>(</m:t>
+                              <m:t>[(</m:t>
                             </m:r>
                             <m:r>
                               <a:rPr lang="en-GB" sz="1400" b="0" i="1">
@@ -28685,7 +28685,19 @@
                                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
-                              <m:t>𝑛𝑇</m:t>
+                              <m:t>𝑛</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t> </m:t>
                             </m:r>
                           </m:sub>
                         </m:sSub>
@@ -28699,6 +28711,430 @@
                             <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
+                          <m:t>+</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑊</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝐸</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>,</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑒𝑛</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>)∙</m:t>
+                        </m:r>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                    <a:solidFill>
+                                      <a:schemeClr val="tx1"/>
+                                    </a:solidFill>
+                                    <a:effectLst/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:cs typeface="+mn-cs"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                    <a:solidFill>
+                                      <a:schemeClr val="tx1"/>
+                                    </a:solidFill>
+                                    <a:effectLst/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:cs typeface="+mn-cs"/>
+                                  </a:rPr>
+                                  <m:t>𝑖</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                    <a:solidFill>
+                                      <a:schemeClr val="tx1"/>
+                                    </a:solidFill>
+                                    <a:effectLst/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:cs typeface="+mn-cs"/>
+                                  </a:rPr>
+                                  <m:t>1,</m:t>
+                                </m:r>
+                                <m:r>
+                                  <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                    <a:solidFill>
+                                      <a:schemeClr val="tx1"/>
+                                    </a:solidFill>
+                                    <a:effectLst/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:cs typeface="+mn-cs"/>
+                                  </a:rPr>
+                                  <m:t>𝑗</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:e>
+                        </m:d>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>+</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>[</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑊</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑑</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t> ∙</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>(</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑊</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑛</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>+</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑊</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝐸</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>,</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑒𝑛</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>)</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>∙</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>(</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝐷</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
                           <m:t>∙</m:t>
                         </m:r>
                         <m:sSub>
@@ -28740,7 +29176,7 @@
                                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
-                              <m:t>1,</m:t>
+                              <m:t>2.1,</m:t>
                             </m:r>
                             <m:r>
                               <a:rPr lang="en-GB" sz="1400" b="0" i="1">
@@ -28766,7 +29202,7 @@
                             <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
-                          <m:t>)+</m:t>
+                          <m:t>+</m:t>
                         </m:r>
                         <m:sSub>
                           <m:sSubPr>
@@ -28793,19 +29229,7 @@
                                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
-                              <m:t>[</m:t>
-                            </m:r>
-                            <m:r>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝑊</m:t>
+                              <m:t>𝐶</m:t>
                             </m:r>
                           </m:e>
                           <m:sub>
@@ -28819,62 +29243,7 @@
                                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
-                              <m:t>𝑑</m:t>
-                            </m:r>
-                          </m:sub>
-                        </m:sSub>
-                        <m:r>
-                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
-                          <m:t> ∙</m:t>
-                        </m:r>
-                        <m:sSub>
-                          <m:sSubPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:sSubPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝑊</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:sub>
-                            <m:r>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝑛𝑇</m:t>
+                              <m:t>𝑆</m:t>
                             </m:r>
                           </m:sub>
                         </m:sSub>
@@ -28890,42 +29259,6 @@
                           </a:rPr>
                           <m:t>∙</m:t>
                         </m:r>
-                        <m:r>
-                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
-                          <m:t>(</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
-                          <m:t>𝐷</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="+mn-ea"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
-                          <m:t>∙</m:t>
-                        </m:r>
                         <m:sSub>
                           <m:sSubPr>
                             <m:ctrlPr>
@@ -28965,7 +29298,7 @@
                                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
-                              <m:t>2.1,</m:t>
+                              <m:t>2.2,</m:t>
                             </m:r>
                             <m:r>
                               <a:rPr lang="en-GB" sz="1400" b="0" i="1">
@@ -29032,7 +29365,7 @@
                                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
-                              <m:t>𝑆</m:t>
+                              <m:t>𝐶</m:t>
                             </m:r>
                           </m:sub>
                         </m:sSub>
@@ -29087,7 +29420,7 @@
                                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
-                              <m:t>2.2,</m:t>
+                              <m:t>2.3,</m:t>
                             </m:r>
                             <m:r>
                               <a:rPr lang="en-GB" sz="1400" b="0" i="1">
@@ -29115,49 +29448,18 @@
                           </a:rPr>
                           <m:t>+</m:t>
                         </m:r>
-                        <m:sSub>
-                          <m:sSubPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:sSubPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝐶</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:sub>
-                            <m:r>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝐶</m:t>
-                            </m:r>
-                          </m:sub>
-                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝐷𝑀</m:t>
+                        </m:r>
                         <m:r>
                           <a:rPr lang="en-GB" sz="1100" b="0" i="1">
                             <a:solidFill>
@@ -29209,7 +29511,7 @@
                                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
-                              <m:t>2.3,</m:t>
+                              <m:t>2.4,</m:t>
                             </m:r>
                             <m:r>
                               <a:rPr lang="en-GB" sz="1400" b="0" i="1">
@@ -29237,30 +29539,6 @@
                           </a:rPr>
                           <m:t>+</m:t>
                         </m:r>
-                        <m:r>
-                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
-                          <m:t>𝐷𝑀</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="+mn-ea"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
-                          <m:t>∙</m:t>
-                        </m:r>
                         <m:sSub>
                           <m:sSubPr>
                             <m:ctrlPr>
@@ -29276,6 +29554,30 @@
                             </m:ctrlPr>
                           </m:sSubPr>
                           <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝐷𝑊</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>∙</m:t>
+                            </m:r>
                             <m:r>
                               <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                                 <a:solidFill>
@@ -29300,7 +29602,7 @@
                                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
-                              <m:t>2.4,</m:t>
+                              <m:t>2.5,</m:t>
                             </m:r>
                             <m:r>
                               <a:rPr lang="en-GB" sz="1400" b="0" i="1">
@@ -29326,7 +29628,7 @@
                             <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
-                          <m:t>+</m:t>
+                          <m:t>+ </m:t>
                         </m:r>
                         <m:sSub>
                           <m:sSubPr>
@@ -29343,30 +29645,6 @@
                             </m:ctrlPr>
                           </m:sSubPr>
                           <m:e>
-                            <m:r>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝐷𝑊</m:t>
-                            </m:r>
-                            <m:r>
-                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>∙</m:t>
-                            </m:r>
                             <m:r>
                               <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                                 <a:solidFill>
@@ -29391,7 +29669,7 @@
                                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
-                              <m:t>2.5,</m:t>
+                              <m:t>2.6</m:t>
                             </m:r>
                             <m:r>
                               <a:rPr lang="en-GB" sz="1400" b="0" i="1">
@@ -29417,73 +29695,6 @@
                             <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
-                          <m:t>+ </m:t>
-                        </m:r>
-                        <m:sSub>
-                          <m:sSubPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:sSubPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝑖</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:sub>
-                            <m:r>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>2.6</m:t>
-                            </m:r>
-                            <m:r>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝑗</m:t>
-                            </m:r>
-                          </m:sub>
-                        </m:sSub>
-                        <m:r>
-                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
                           <m:t>)]+(</m:t>
                         </m:r>
                         <m:sSub>
@@ -29525,31 +29736,7 @@
                                 <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
-                              <m:t>𝑛𝑇</m:t>
-                            </m:r>
-                            <m:r>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>−</m:t>
-                            </m:r>
-                            <m:r>
-                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝑒</m:t>
+                              <m:t>𝑛</m:t>
                             </m:r>
                           </m:sub>
                         </m:sSub>
@@ -30257,49 +30444,18 @@
                               </a:rPr>
                               <m:t>1−</m:t>
                             </m:r>
-                            <m:sSub>
-                              <m:sSubPr>
-                                <m:ctrlPr>
-                                  <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                    <a:solidFill>
-                                      <a:schemeClr val="tx1"/>
-                                    </a:solidFill>
-                                    <a:effectLst/>
-                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                    <a:ea typeface="+mn-ea"/>
-                                    <a:cs typeface="+mn-cs"/>
-                                  </a:rPr>
-                                </m:ctrlPr>
-                              </m:sSubPr>
-                              <m:e>
-                                <m:r>
-                                  <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                    <a:solidFill>
-                                      <a:schemeClr val="tx1"/>
-                                    </a:solidFill>
-                                    <a:effectLst/>
-                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                    <a:ea typeface="+mn-ea"/>
-                                    <a:cs typeface="+mn-cs"/>
-                                  </a:rPr>
-                                  <m:t>𝐴</m:t>
-                                </m:r>
-                              </m:e>
-                              <m:sub>
-                                <m:r>
-                                  <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                                    <a:solidFill>
-                                      <a:schemeClr val="tx1"/>
-                                    </a:solidFill>
-                                    <a:effectLst/>
-                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                    <a:ea typeface="+mn-ea"/>
-                                    <a:cs typeface="+mn-cs"/>
-                                  </a:rPr>
-                                  <m:t>𝑃</m:t>
-                                </m:r>
-                              </m:sub>
-                            </m:sSub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝐴𝑃</m:t>
+                            </m:r>
                           </m:e>
                         </m:d>
                         <m:r>
@@ -30470,7 +30626,31 @@
                             <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
-                          <m:t>∙1000∙30)</m:t>
+                          <m:t>∙1000∙</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝐿𝑇</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>)</m:t>
                         </m:r>
                       </m:den>
                     </m:f>
@@ -30642,7 +30822,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="33" name="TextBox 32">
@@ -30656,8 +30836,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="215409" y="2017210"/>
-              <a:ext cx="17882092" cy="479427"/>
+              <a:off x="215409" y="2074937"/>
+              <a:ext cx="17882092" cy="502382"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -30706,7 +30886,7 @@
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t> (〖(𝑊〗_𝑛𝑇∙𝑖_(1,𝑗))+〖[𝑊〗_𝑑  ∙𝑊_𝑛𝑇</a:t>
+                <a:t> (〖[(𝑊〗_(𝑛 )+𝑊_(𝐸,𝑒𝑛))∙(𝑖_(1,𝑗) )+〖[𝑊〗_𝑑  ∙〖(𝑊〗_𝑛+𝑊_(𝐸,𝑒𝑛))</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
@@ -30850,7 +31030,7 @@
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>𝑖〗_(2.5,𝑗)+ 𝑖_2.6𝑗)]+(𝑊_(𝑛𝑇−𝑒)</a:t>
+                <a:t>𝑖〗_(2.5,𝑗)+ 𝑖_2.6𝑗)]+(𝑊_𝑛</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
@@ -30934,7 +31114,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>𝑃_(𝑛,𝑒)∙𝐶𝐹∙(1−𝐴_𝑃 )∙𝐿𝑇∙ 8760000]−(</a:t>
+                <a:t>𝑃_(𝑛,𝑒)∙𝐶𝐹∙(1−𝐴𝑃)∙𝐿𝑇∙ 8760000]−(</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
@@ -30958,7 +31138,7 @@
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>∙1000∙30)) </a:t>
+                <a:t>∙1000∙𝐿𝑇)) </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1400" b="0" i="0">
@@ -31563,13 +31743,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>13417078</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>189108</xdr:rowOff>
+      <xdr:colOff>13444292</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>121074</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4003275" cy="225190"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="3914405" cy="336246"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="36" name="TextBox 35">
@@ -31583,8 +31763,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13417078" y="5852153"/>
-              <a:ext cx="4003275" cy="225190"/>
+              <a:off x="13444292" y="7305645"/>
+              <a:ext cx="3914405" cy="336246"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -31689,45 +31869,89 @@
                     <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                       <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                     </a:rPr>
-                    <m:t>=  </m:t>
+                    <m:t>= </m:t>
                   </m:r>
-                  <m:sSub>
-                    <m:sSubPr>
+                  <m:f>
+                    <m:fPr>
                       <m:ctrlPr>
                         <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
                       </m:ctrlPr>
-                    </m:sSubPr>
-                    <m:e>
+                    </m:fPr>
+                    <m:num>
+                      <m:sSub>
+                        <m:sSubPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSubPr>
+                        <m:e>
+                          <m:r>
+                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                            <m:t>𝑊</m:t>
+                          </m:r>
+                        </m:e>
+                        <m:sub>
+                          <m:r>
+                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                            <m:t>𝐸</m:t>
+                          </m:r>
+                          <m:r>
+                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                            <m:t>, </m:t>
+                          </m:r>
+                          <m:r>
+                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                            <m:t>𝑛</m:t>
+                          </m:r>
+                        </m:sub>
+                      </m:sSub>
+                    </m:num>
+                    <m:den>
                       <m:r>
                         <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
-                        <m:t>𝑊</m:t>
+                        <m:t>𝑆</m:t>
                       </m:r>
-                    </m:e>
-                    <m:sub>
-                      <m:r>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝐸</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>, </m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑛</m:t>
-                      </m:r>
-                    </m:sub>
-                  </m:sSub>
+                      <m:sSub>
+                        <m:sSubPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSubPr>
+                        <m:e>
+                          <m:r>
+                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                            <m:t>𝑅</m:t>
+                          </m:r>
+                        </m:e>
+                        <m:sub>
+                          <m:r>
+                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
+                            <m:t>𝐸</m:t>
+                          </m:r>
+                        </m:sub>
+                      </m:sSub>
+                    </m:den>
+                  </m:f>
                   <m:r>
                     <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                       <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -31742,13 +31966,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="36" name="TextBox 35">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAFC5192-8EC0-491B-98D4-FF21664B1B72}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000024000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -31756,8 +31980,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13417078" y="5852153"/>
-              <a:ext cx="4003275" cy="225190"/>
+              <a:off x="13444292" y="7305645"/>
+              <a:ext cx="3914405" cy="336246"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -31809,7 +32033,7 @@
                 <a:rPr lang="en-GB" sz="1400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑊_(𝐸,𝑒𝑛)=  𝑊_(𝐸, 𝑛)</a:t>
+                <a:t>𝑊_(𝐸,𝑒𝑛)=  𝑊_(𝐸, 𝑛)/(𝑆𝑅_𝐸 )</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1400" b="0" i="0">
@@ -32319,8 +32543,8 @@
       <xdr:rowOff>184945</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4936021" cy="274498"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="38" name="TextBox 37">
@@ -32405,7 +32629,7 @@
                         <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
-                        <m:t>𝑛𝑇</m:t>
+                        <m:t>𝑛</m:t>
                       </m:r>
                     </m:sub>
                   </m:sSub>
@@ -32636,13 +32860,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="38" name="TextBox 37">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000026000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -32696,7 +32920,7 @@
                 <a:rPr lang="en-GB" sz="1400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>: 𝑊_𝑛𝑇=  𝑊_(𝑃, 𝑛)  [ 1+1⁄</a:t>
+                <a:t>: 𝑊_𝑛=  𝑊_(𝑃, 𝑛)  [ 1+1⁄</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
@@ -32797,8 +33021,8 @@
       <xdr:rowOff>60933</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4545341" cy="486458"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="49" name="TextBox 48">
@@ -32883,7 +33107,7 @@
                         <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
-                        <m:t>𝑛𝑇</m:t>
+                        <m:t>𝑛</m:t>
                       </m:r>
                     </m:sub>
                   </m:sSub>
@@ -33199,137 +33423,6 @@
                       </m:f>
                     </m:e>
                   </m:d>
-                  <m:r>
-                    <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                    </a:rPr>
-                    <m:t>+ </m:t>
-                  </m:r>
-                  <m:f>
-                    <m:fPr>
-                      <m:ctrlPr>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                      </m:ctrlPr>
-                    </m:fPr>
-                    <m:num>
-                      <m:sSub>
-                        <m:sSubPr>
-                          <m:ctrlPr>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:solidFill>
-                                <a:schemeClr val="tx1"/>
-                              </a:solidFill>
-                              <a:effectLst/>
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              <a:ea typeface="+mn-ea"/>
-                              <a:cs typeface="+mn-cs"/>
-                            </a:rPr>
-                          </m:ctrlPr>
-                        </m:sSubPr>
-                        <m:e>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:solidFill>
-                                <a:schemeClr val="tx1"/>
-                              </a:solidFill>
-                              <a:effectLst/>
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              <a:ea typeface="+mn-ea"/>
-                              <a:cs typeface="+mn-cs"/>
-                            </a:rPr>
-                            <m:t>𝑊</m:t>
-                          </m:r>
-                        </m:e>
-                        <m:sub>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:solidFill>
-                                <a:schemeClr val="tx1"/>
-                              </a:solidFill>
-                              <a:effectLst/>
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              <a:ea typeface="+mn-ea"/>
-                              <a:cs typeface="+mn-cs"/>
-                            </a:rPr>
-                            <m:t>𝐸</m:t>
-                          </m:r>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:solidFill>
-                                <a:schemeClr val="tx1"/>
-                              </a:solidFill>
-                              <a:effectLst/>
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              <a:ea typeface="+mn-ea"/>
-                              <a:cs typeface="+mn-cs"/>
-                            </a:rPr>
-                            <m:t>,</m:t>
-                          </m:r>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:solidFill>
-                                <a:schemeClr val="tx1"/>
-                              </a:solidFill>
-                              <a:effectLst/>
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              <a:ea typeface="+mn-ea"/>
-                              <a:cs typeface="+mn-cs"/>
-                            </a:rPr>
-                            <m:t>𝑒𝑛</m:t>
-                          </m:r>
-                        </m:sub>
-                      </m:sSub>
-                    </m:num>
-                    <m:den>
-                      <m:sSub>
-                        <m:sSubPr>
-                          <m:ctrlPr>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:solidFill>
-                                <a:schemeClr val="tx1"/>
-                              </a:solidFill>
-                              <a:effectLst/>
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              <a:ea typeface="+mn-ea"/>
-                              <a:cs typeface="+mn-cs"/>
-                            </a:rPr>
-                          </m:ctrlPr>
-                        </m:sSubPr>
-                        <m:e>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:solidFill>
-                                <a:schemeClr val="tx1"/>
-                              </a:solidFill>
-                              <a:effectLst/>
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              <a:ea typeface="+mn-ea"/>
-                              <a:cs typeface="+mn-cs"/>
-                            </a:rPr>
-                            <m:t>𝑆𝑅</m:t>
-                          </m:r>
-                        </m:e>
-                        <m:sub>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:solidFill>
-                                <a:schemeClr val="tx1"/>
-                              </a:solidFill>
-                              <a:effectLst/>
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              <a:ea typeface="+mn-ea"/>
-                              <a:cs typeface="+mn-cs"/>
-                            </a:rPr>
-                            <m:t>𝐸</m:t>
-                          </m:r>
-                        </m:sub>
-                      </m:sSub>
-                    </m:den>
-                  </m:f>
                 </m:oMath>
               </a14:m>
               <a:r>
@@ -33340,13 +33433,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="49" name="TextBox 48">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000031000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -33400,7 +33493,7 @@
                 <a:rPr lang="en-GB" sz="1400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>: 𝑊_𝑛𝑇=  𝑊_(𝑃, 𝑛) ((1+ </a:t>
+                <a:t>: 𝑊_𝑛=  𝑊_(𝑃, 𝑛) ((1+ </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1100" b="0" i="0">
@@ -33474,49 +33567,6 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
                 <a:t>〖𝑆𝑅〗_𝑀 )</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>+ </a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t> 𝑊_(𝐸,𝑒𝑛)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>/</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>〖𝑆𝑅〗_𝐸 </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1400"/>
@@ -33656,331 +33706,6 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>323896</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>178346</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3669338" cy="336246"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="60" name="TextBox 59">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003C000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="323896" y="7893596"/>
-              <a:ext cx="3669338" cy="336246"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>Total</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1400" b="0" i="1" baseline="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t> number w/o expl</a:t>
-              </a:r>
-              <a14:m>
-                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:r>
-                    <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                    </a:rPr>
-                    <m:t>: </m:t>
-                  </m:r>
-                  <m:sSub>
-                    <m:sSubPr>
-                      <m:ctrlPr>
-                        <a:rPr lang="en-GB" sz="1400" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                      </m:ctrlPr>
-                    </m:sSubPr>
-                    <m:e>
-                      <m:r>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑊</m:t>
-                      </m:r>
-                    </m:e>
-                    <m:sub>
-                      <m:r>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑛𝑇</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>−</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑒</m:t>
-                      </m:r>
-                    </m:sub>
-                  </m:sSub>
-                  <m:r>
-                    <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                    </a:rPr>
-                    <m:t>=  </m:t>
-                  </m:r>
-                  <m:sSub>
-                    <m:sSubPr>
-                      <m:ctrlPr>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                      </m:ctrlPr>
-                    </m:sSubPr>
-                    <m:e>
-                      <m:r>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑊</m:t>
-                      </m:r>
-                    </m:e>
-                    <m:sub>
-                      <m:r>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑛𝑇</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>,</m:t>
-                      </m:r>
-                    </m:sub>
-                  </m:sSub>
-                  <m:r>
-                    <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                    </a:rPr>
-                    <m:t>−</m:t>
-                  </m:r>
-                  <m:f>
-                    <m:fPr>
-                      <m:ctrlPr>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                      </m:ctrlPr>
-                    </m:fPr>
-                    <m:num>
-                      <m:sSub>
-                        <m:sSubPr>
-                          <m:ctrlPr>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                          </m:ctrlPr>
-                        </m:sSubPr>
-                        <m:e>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                            <m:t>𝑊</m:t>
-                          </m:r>
-                        </m:e>
-                        <m:sub>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                            <m:t>𝐸</m:t>
-                          </m:r>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                            <m:t>,</m:t>
-                          </m:r>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                            <m:t>𝑒𝑛</m:t>
-                          </m:r>
-                        </m:sub>
-                      </m:sSub>
-                    </m:num>
-                    <m:den>
-                      <m:r>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑆</m:t>
-                      </m:r>
-                      <m:sSub>
-                        <m:sSubPr>
-                          <m:ctrlPr>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                          </m:ctrlPr>
-                        </m:sSubPr>
-                        <m:e>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                            <m:t>𝑅</m:t>
-                          </m:r>
-                        </m:e>
-                        <m:sub>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                            <m:t>𝐸</m:t>
-                          </m:r>
-                        </m:sub>
-                      </m:sSub>
-                    </m:den>
-                  </m:f>
-                  <m:r>
-                    <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                    </a:rPr>
-                    <m:t> </m:t>
-                  </m:r>
-                </m:oMath>
-              </a14:m>
-              <a:endParaRPr lang="en-GB" sz="1400"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="60" name="TextBox 59">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003C000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="323896" y="7893596"/>
-              <a:ext cx="3669338" cy="336246"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>Total</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1400" b="0" i="1" baseline="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t> number w/o expl</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>: 𝑊_(𝑛𝑇−𝑒)=  𝑊_(𝑛𝑇,)−𝑊_(𝐸,𝑒𝑛)/(𝑆𝑅_𝐸 )</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>  </a:t>
-              </a:r>
-              <a:endParaRPr lang="en-GB" sz="1400"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>6761512</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>55253</xdr:rowOff>
@@ -34052,8 +33777,8 @@
       <xdr:rowOff>126471</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3464143" cy="377794"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="41" name="TextBox 40">
@@ -34138,7 +33863,7 @@
                         <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
-                        <m:t>𝑛𝑇</m:t>
+                        <m:t>𝑛</m:t>
                       </m:r>
                     </m:sub>
                   </m:sSub>
@@ -34241,13 +33966,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="41" name="TextBox 40">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000029000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -34301,7 +34026,7 @@
                 <a:rPr lang="en-GB" sz="1400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>: 𝑊_𝑛𝑇=  𝑊_(𝑃𝐼, 𝑛)</a:t>
+                <a:t>: 𝑊_𝑛=  𝑊_(𝑃𝐼, 𝑛)</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1400" b="0" i="0">
@@ -34321,9 +34046,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7148488</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>164119</xdr:rowOff>
+      <xdr:colOff>13244488</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>109690</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1860509" cy="374141"/>
     <xdr:sp macro="" textlink="">
@@ -34339,7 +34064,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7148488" y="5632590"/>
+          <a:off x="13244488" y="6899654"/>
           <a:ext cx="1860509" cy="374141"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -35069,19 +34794,85 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7211654</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>40015</xdr:rowOff>
+      <xdr:colOff>13239750</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>149678</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3677995" cy="336246"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <xdr:ext cx="2188484" cy="374141"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="TextBox 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13239750" y="6000749"/>
+          <a:ext cx="2188484" cy="374141"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1"/>
+            <a:t>Without</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1" baseline="0"/>
+            <a:t> s</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1"/>
+            <a:t>uccess rate</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>13447012</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>151009</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3963714" cy="225190"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="48" name="TextBox 47">
+            <xdr:cNvPr id="54" name="TextBox 53">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000030000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000024000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -35089,8 +34880,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7211654" y="6337098"/>
-              <a:ext cx="3677995" cy="336246"/>
+              <a:off x="13447012" y="6559973"/>
+              <a:ext cx="3963714" cy="225190"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -35122,22 +34913,37 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>Total</a:t>
+                <a:t>Equivalent</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1400" b="0" i="1" baseline="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t> number w/o expl</a:t>
+                <a:t> exploratory</a:t>
               </a:r>
               <a14:m>
                 <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:r>
                     <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                       <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                     </a:rPr>
-                    <m:t>: </m:t>
+                    <m:t> </m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>𝑤𝑒𝑙𝑙𝑠</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-GB" sz="1400" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t> : </m:t>
                   </m:r>
                   <m:sSub>
                     <m:sSubPr>
@@ -35160,19 +34966,19 @@
                         <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
-                        <m:t>𝑛𝑇</m:t>
+                        <m:t>𝐸</m:t>
                       </m:r>
                       <m:r>
                         <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
-                        <m:t>−</m:t>
+                        <m:t>,</m:t>
                       </m:r>
                       <m:r>
                         <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
-                        <m:t>𝑒</m:t>
+                        <m:t>𝑒𝑛</m:t>
                       </m:r>
                     </m:sub>
                   </m:sSub>
@@ -35180,20 +34986,32 @@
                     <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                       <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                     </a:rPr>
-                    <m:t>=  </m:t>
+                    <m:t>= </m:t>
                   </m:r>
                   <m:sSub>
                     <m:sSubPr>
                       <m:ctrlPr>
                         <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
                         </a:rPr>
                       </m:ctrlPr>
                     </m:sSubPr>
                     <m:e>
                       <m:r>
                         <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
                         </a:rPr>
                         <m:t>𝑊</m:t>
                       </m:r>
@@ -35201,19 +35019,37 @@
                     <m:sub>
                       <m:r>
                         <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
                         </a:rPr>
-                        <m:t>𝑇</m:t>
+                        <m:t>𝐸</m:t>
                       </m:r>
                       <m:r>
                         <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
                         </a:rPr>
                         <m:t>, </m:t>
                       </m:r>
                       <m:r>
                         <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
                         </a:rPr>
                         <m:t>𝑛</m:t>
                       </m:r>
@@ -35222,96 +35058,9 @@
                   <m:r>
                     <a:rPr lang="en-GB" sz="1400" b="0" i="1">
                       <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                    </a:rPr>
-                    <m:t>−</m:t>
-                  </m:r>
-                  <m:f>
-                    <m:fPr>
-                      <m:ctrlPr>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                      </m:ctrlPr>
-                    </m:fPr>
-                    <m:num>
-                      <m:sSub>
-                        <m:sSubPr>
-                          <m:ctrlPr>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                          </m:ctrlPr>
-                        </m:sSubPr>
-                        <m:e>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                            <m:t>𝑊</m:t>
-                          </m:r>
-                        </m:e>
-                        <m:sub>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                            <m:t>𝐸</m:t>
-                          </m:r>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                            <m:t>, </m:t>
-                          </m:r>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                            <m:t>𝑒𝑛</m:t>
-                          </m:r>
-                        </m:sub>
-                      </m:sSub>
-                    </m:num>
-                    <m:den>
-                      <m:r>
-                        <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑆</m:t>
-                      </m:r>
-                      <m:sSub>
-                        <m:sSubPr>
-                          <m:ctrlPr>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                          </m:ctrlPr>
-                        </m:sSubPr>
-                        <m:e>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                            <m:t>𝑅</m:t>
-                          </m:r>
-                        </m:e>
-                        <m:sub>
-                          <m:r>
-                            <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            </a:rPr>
-                            <m:t>𝐸</m:t>
-                          </m:r>
-                        </m:sub>
-                      </m:sSub>
-                    </m:den>
-                  </m:f>
-                  <m:r>
-                    <a:rPr lang="en-GB" sz="1400" b="0" i="1">
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                     </a:rPr>
-                    <m:t> </m:t>
+                    <m:t>×0.3 </m:t>
                   </m:r>
                 </m:oMath>
               </a14:m>
@@ -35320,13 +35069,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="48" name="TextBox 47">
+            <xdr:cNvPr id="54" name="TextBox 53">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000030000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000024000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -35334,8 +35083,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7211654" y="6337098"/>
-              <a:ext cx="3677995" cy="336246"/>
+              <a:off x="13447012" y="6559973"/>
+              <a:ext cx="3963714" cy="225190"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -35367,27 +35116,46 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>Total</a:t>
+                <a:t>Equivalent</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1400" b="0" i="1" baseline="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t> number w/o expl</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>: 𝑊_(𝑛𝑇−𝑒)=  𝑊_(𝑇, 𝑛)−𝑊_(𝐸, 𝑒𝑛)/(𝑆𝑅_𝐸 )</a:t>
+                <a:t> exploratory</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-GB" sz="1400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>  </a:t>
+                <a:t> 𝑤𝑒𝑙𝑙𝑠 : </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑊_(𝐸,𝑒𝑛)= </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑊_(𝐸, 𝑛)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>×0.3 </a:t>
               </a:r>
               <a:endParaRPr lang="en-GB" sz="1400"/>
             </a:p>
@@ -35395,6 +35163,64 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6912428</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1860509" cy="374141"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="TextBox 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6912428" y="5660571"/>
+          <a:ext cx="1860509" cy="374141"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1"/>
+            <a:t>With success rate</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
@@ -35699,7 +35525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -35728,8 +35554,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>